<commit_message>
Final version of presentation
</commit_message>
<xml_diff>
--- a/result_set.xlsx
+++ b/result_set.xlsx
@@ -647,34 +647,34 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.47</v>
+        <v>0.23</v>
       </c>
       <c r="V2" t="n">
-        <v>0.51</v>
+        <v>0.35</v>
       </c>
       <c r="W2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.02</v>
       </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AC2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AD2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3">
@@ -742,31 +742,31 @@
         <v>0.23</v>
       </c>
       <c r="V3" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="W3" t="n">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="X3" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="Z3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AB3" t="n">
         <v>0.01</v>
       </c>
-      <c r="AA3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0</v>
-      </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4">
@@ -834,7 +834,7 @@
         <v>0.93</v>
       </c>
       <c r="V4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -923,31 +923,31 @@
         <v>0.109</v>
       </c>
       <c r="U5" t="n">
-        <v>0.11</v>
+        <v>0.23</v>
       </c>
       <c r="V5" t="n">
-        <v>0.18</v>
+        <v>0.35</v>
       </c>
       <c r="W5" t="n">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="X5" t="n">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AD5" t="n">
         <v>0.01</v>

</xml_diff>

<commit_message>
Monte Carlo for AI notebook created
</commit_message>
<xml_diff>
--- a/result_set.xlsx
+++ b/result_set.xlsx
@@ -647,34 +647,34 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
       <c r="V2" t="n">
-        <v>0.35</v>
+        <v>0.51</v>
       </c>
       <c r="W2" t="n">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
       <c r="X2" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -739,34 +739,34 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="V3" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="W3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="X3" t="n">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -834,10 +834,10 @@
         <v>0.93</v>
       </c>
       <c r="V4" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -923,31 +923,31 @@
         <v>0.109</v>
       </c>
       <c r="U5" t="n">
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="V5" t="n">
-        <v>0.35</v>
+        <v>0.18</v>
       </c>
       <c r="W5" t="n">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="X5" t="n">
-        <v>0.12</v>
+        <v>0.22</v>
       </c>
       <c r="Y5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="AA5" t="n">
         <v>0.05</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AB5" t="n">
         <v>0.03</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AC5" t="n">
         <v>0.02</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.01</v>
       </c>
       <c r="AD5" t="n">
         <v>0.01</v>

</xml_diff>

<commit_message>
Softmax addes to leanr from simulation experiment (_modern extension)
</commit_message>
<xml_diff>
--- a/result_set.xlsx
+++ b/result_set.xlsx
@@ -647,10 +647,10 @@
         <v>0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.47</v>
+        <v>0.59</v>
       </c>
       <c r="V2" t="n">
-        <v>0.51</v>
+        <v>0.36</v>
       </c>
       <c r="W2" t="n">
         <v>0.02</v>
@@ -739,25 +739,25 @@
         <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="V3" t="n">
-        <v>0.44</v>
+        <v>0.42</v>
       </c>
       <c r="W3" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="X3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="Z3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="AA3" t="n">
         <v>0.01</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>0</v>
       </c>
       <c r="AB3" t="n">
         <v>0</v>
@@ -831,13 +831,13 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="V4" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>

</xml_diff>